<commit_message>
feat: implement sell data creation in CreateSellView and clean up unused search function in sell_controller
</commit_message>
<xml_diff>
--- a/src/business/data/sell_data.xlsx
+++ b/src/business/data/sell_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,7 +524,49 @@
         <v>1200000</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>45814.02324728566</v>
+        <v>45814.02324728009</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2AYB-3AYB-5AYB</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1-1-1</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>27500</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>45815.77188895833</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1AYB-1AP-1M</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2-3-2</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>45700</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>45815.77444396124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: enhance sell data handling with improved Excel formatting and detail view in ManageSellView
</commit_message>
<xml_diff>
--- a/src/business/data/sell_data.xlsx
+++ b/src/business/data/sell_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,103 +470,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AB1-AB2-AB3</t>
+          <t>1AYB-5AYB-1AP-1M-4AYB</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1-4-10</t>
+          <t>1-1-1-1-1</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>54200</v>
+        <v>32100</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45814.0092422801</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>AB4-AB5-AB10</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>20-5-10</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>68100</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>45814.02255357639</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>AB5-CA5-TA1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>40-50-60</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1200000</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>45814.02324728009</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2AYB-3AYB-5AYB</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1-1-1</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>27500</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>45815.77188895833</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1AYB-1AP-1M</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2-3-2</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>45700</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>45815.77444396124</v>
+        <v>45815.80757366943</v>
       </c>
     </row>
   </sheetData>

</xml_diff>